<commit_message>
Update crypto analysis scripts and fix file path in MT54XCConnection.py
</commit_message>
<xml_diff>
--- a/D-Advance_Technical_Analysis_KMI100_STRONG_BUY.xlsx
+++ b/D-Advance_Technical_Analysis_KMI100_STRONG_BUY.xlsx
@@ -667,7 +667,7 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -733,7 +733,7 @@
     </row>
     <row r="3">
       <c r="A3" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -799,7 +799,7 @@
     </row>
     <row r="4">
       <c r="A4" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
     </row>
     <row r="5">
       <c r="A5" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -931,7 +931,7 @@
     </row>
     <row r="6">
       <c r="A6" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -997,7 +997,7 @@
     </row>
     <row r="7">
       <c r="A7" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="8">
       <c r="A8" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="9">
       <c r="A9" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="10">
       <c r="A10" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="11">
       <c r="A11" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="12">
       <c r="A12" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="13">
       <c r="A13" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="14">
       <c r="A14" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="15">
       <c r="A15" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="16">
       <c r="A16" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="17">
       <c r="A17" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="18">
       <c r="A18" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1789,7 +1789,7 @@
     </row>
     <row r="19">
       <c r="A19" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="20">
       <c r="A20" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1921,7 +1921,7 @@
     </row>
     <row r="21">
       <c r="A21" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="22">
       <c r="A22" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="23">
       <c r="A23" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="24">
       <c r="A24" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="25">
       <c r="A25" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="26">
       <c r="A26" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="27">
       <c r="A27" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="28">
       <c r="A28" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="29">
       <c r="A29" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="30">
       <c r="A30" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="31">
       <c r="A31" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="32">
       <c r="A32" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2713,7 +2713,7 @@
     </row>
     <row r="33">
       <c r="A33" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="34">
       <c r="A34" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="35">
       <c r="A35" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2911,7 +2911,7 @@
     </row>
     <row r="36">
       <c r="A36" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -2977,7 +2977,7 @@
     </row>
     <row r="37">
       <c r="A37" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="38">
       <c r="A38" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="39">
       <c r="A39" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3175,7 +3175,7 @@
     </row>
     <row r="40">
       <c r="A40" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="41">
       <c r="A41" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3307,7 +3307,7 @@
     </row>
     <row r="42">
       <c r="A42" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3373,7 +3373,7 @@
     </row>
     <row r="43">
       <c r="A43" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3439,7 +3439,7 @@
     </row>
     <row r="44">
       <c r="A44" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="45">
       <c r="A45" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="46">
       <c r="A46" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="47">
       <c r="A47" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="48">
       <c r="A48" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -3769,7 +3769,7 @@
     </row>
     <row r="49">
       <c r="A49" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="50">
       <c r="A50" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -3901,7 +3901,7 @@
     </row>
     <row r="51">
       <c r="A51" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="52">
       <c r="A52" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="53">
       <c r="A53" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -4099,7 +4099,7 @@
     </row>
     <row r="54">
       <c r="A54" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -4165,7 +4165,7 @@
     </row>
     <row r="55">
       <c r="A55" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="56">
       <c r="A56" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -4297,7 +4297,7 @@
     </row>
     <row r="57">
       <c r="A57" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4363,7 +4363,7 @@
     </row>
     <row r="58">
       <c r="A58" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="59">
       <c r="A59" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="60">
       <c r="A60" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -4561,7 +4561,7 @@
     </row>
     <row r="61">
       <c r="A61" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="62">
       <c r="A62" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -4693,7 +4693,7 @@
     </row>
     <row r="63">
       <c r="A63" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -4779,7 +4779,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4884,77 +4884,77 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NRSL</t>
+          <t>KOHC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>STRONG_BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>20.23</v>
+        <v>277.67</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" t="n">
-        <v>224183</v>
+        <v>586102</v>
       </c>
       <c r="I2" t="n">
-        <v>30.73140543580916</v>
+        <v>45.96840354445689</v>
       </c>
       <c r="J2" s="8" t="n">
-        <v>64.31171952233328</v>
+        <v>75.96599585177277</v>
       </c>
       <c r="K2" t="n">
-        <v>59.77654959241123</v>
+        <v>79.14158399414431</v>
       </c>
       <c r="L2" s="8" t="n">
-        <v>0.8938235294117938</v>
+        <v>43.25955882352952</v>
       </c>
       <c r="M2" t="n">
-        <v>1.914357682619642</v>
+        <v>-0.8321428571428514</v>
       </c>
       <c r="N2" t="n">
-        <v>16.52944444444445</v>
+        <v>194.6172222222222</v>
       </c>
       <c r="O2" t="n">
-        <v>21.69944444444444</v>
+        <v>282.6172222222222</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ANRSL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AKOHC</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-NRSL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-KOHC/financials-overview/</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-NRSL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-KOHC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>KOHC</t>
+          <t>CPHL</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -4963,64 +4963,64 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>277.67</v>
+        <v>31.95</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G3" t="n">
         <v>14</v>
       </c>
       <c r="H3" t="n">
-        <v>586102</v>
+        <v>1697677</v>
       </c>
       <c r="I3" t="n">
-        <v>45.96840354445689</v>
+        <v>24.98440791809918</v>
       </c>
       <c r="J3" s="8" t="n">
-        <v>75.96599585177277</v>
+        <v>61.21963527856168</v>
       </c>
       <c r="K3" t="n">
-        <v>79.14158399414431</v>
+        <v>64.70382229713717</v>
       </c>
       <c r="L3" s="8" t="n">
-        <v>43.25955882352952</v>
+        <v>2.844176470588174</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.8321428571428514</v>
+        <v>-1.510480887792844</v>
       </c>
       <c r="N3" t="n">
-        <v>194.6172222222222</v>
+        <v>26.43444444444445</v>
       </c>
       <c r="O3" t="n">
-        <v>282.6172222222222</v>
+        <v>30.44944444444444</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AKOHC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ACPHL</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-KOHC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-CPHL/financials-overview/</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-KOHC/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-CPHL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CPHL</t>
+          <t>PABC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -5029,64 +5029,64 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>31.95</v>
+        <v>75.98999999999999</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" t="n">
-        <v>1697677</v>
+        <v>1029315</v>
       </c>
       <c r="I4" t="n">
-        <v>24.98440791809918</v>
+        <v>20.31190401707754</v>
       </c>
       <c r="J4" s="8" t="n">
-        <v>61.21963527856168</v>
+        <v>62.74527517100422</v>
       </c>
       <c r="K4" t="n">
-        <v>64.70382229713717</v>
+        <v>61.44243158837864</v>
       </c>
       <c r="L4" s="8" t="n">
-        <v>2.844176470588174</v>
+        <v>2.090647058823606</v>
       </c>
       <c r="M4" t="n">
-        <v>-1.510480887792844</v>
+        <v>0.769128762763557</v>
       </c>
       <c r="N4" t="n">
-        <v>26.43444444444445</v>
+        <v>67.55555555555556</v>
       </c>
       <c r="O4" t="n">
-        <v>30.44944444444444</v>
+        <v>78.55555555555556</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ACPHL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APABC</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-CPHL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PABC/financials-overview/</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-CPHL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PABC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PABC</t>
+          <t>PAEL</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -5095,64 +5095,64 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>75.98999999999999</v>
+        <v>25.49</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H5" t="n">
-        <v>1029315</v>
+        <v>5599157</v>
       </c>
       <c r="I5" t="n">
-        <v>20.31190401707754</v>
+        <v>16.97528834220062</v>
       </c>
       <c r="J5" s="8" t="n">
-        <v>62.74527517100422</v>
+        <v>51.00091281209864</v>
       </c>
       <c r="K5" t="n">
-        <v>61.44243158837864</v>
+        <v>56.60698881510402</v>
       </c>
       <c r="L5" s="8" t="n">
-        <v>2.090647058823606</v>
+        <v>0.9227941176470438</v>
       </c>
       <c r="M5" t="n">
-        <v>0.769128762763557</v>
+        <v>-2.337164750957866</v>
       </c>
       <c r="N5" t="n">
-        <v>67.55555555555556</v>
+        <v>22.30833333333334</v>
       </c>
       <c r="O5" t="n">
-        <v>78.55555555555556</v>
+        <v>27.27666666666667</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APABC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APAEL</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PABC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PAEL/financials-overview/</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PABC/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PAEL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PAEL</t>
+          <t>PIOC</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -5161,64 +5161,64 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>25.49</v>
+        <v>178.75</v>
       </c>
       <c r="E6" t="n">
         <v>5</v>
       </c>
       <c r="F6" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G6" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H6" t="n">
-        <v>5599157</v>
+        <v>118668</v>
       </c>
       <c r="I6" t="n">
-        <v>16.97528834220062</v>
+        <v>26.97168692097832</v>
       </c>
       <c r="J6" s="8" t="n">
-        <v>51.00091281209864</v>
+        <v>66.43928143411412</v>
       </c>
       <c r="K6" t="n">
-        <v>56.60698881510402</v>
+        <v>70.81171884051835</v>
       </c>
       <c r="L6" s="8" t="n">
-        <v>0.9227941176470438</v>
+        <v>14.27126470588234</v>
       </c>
       <c r="M6" t="n">
-        <v>-2.337164750957866</v>
+        <v>-1.237637438532521</v>
       </c>
       <c r="N6" t="n">
-        <v>22.30833333333334</v>
+        <v>135.0205555555556</v>
       </c>
       <c r="O6" t="n">
-        <v>27.27666666666667</v>
+        <v>188.9938888888889</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APAEL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APIOC</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PAEL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PIOC/financials-overview/</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PAEL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PIOC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PIOC</t>
+          <t>TGL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -5227,64 +5227,64 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>178.75</v>
+        <v>116.06</v>
       </c>
       <c r="E7" t="n">
         <v>5</v>
       </c>
       <c r="F7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H7" t="n">
-        <v>118668</v>
+        <v>168359</v>
       </c>
       <c r="I7" t="n">
-        <v>26.97168692097832</v>
+        <v>37.321931890146</v>
       </c>
       <c r="J7" s="8" t="n">
-        <v>66.43928143411412</v>
+        <v>53.20552127078303</v>
       </c>
       <c r="K7" t="n">
-        <v>70.81171884051835</v>
+        <v>56.54715548848657</v>
       </c>
       <c r="L7" s="8" t="n">
-        <v>14.27126470588234</v>
+        <v>2.703323529411662</v>
       </c>
       <c r="M7" t="n">
-        <v>-1.237637438532521</v>
+        <v>-0.8796652147920412</v>
       </c>
       <c r="N7" t="n">
-        <v>135.0205555555556</v>
+        <v>96.84166666666668</v>
       </c>
       <c r="O7" t="n">
-        <v>188.9938888888889</v>
+        <v>133.875</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APIOC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ATGL</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PIOC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-TGL/financials-overview/</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PIOC/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-TGL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TGL</t>
+          <t>PPL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -5293,130 +5293,130 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>116.06</v>
+        <v>120.82</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" t="n">
         <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" t="n">
-        <v>168359</v>
+        <v>2447648</v>
       </c>
       <c r="I8" t="n">
-        <v>37.321931890146</v>
+        <v>17.79431331633835</v>
       </c>
       <c r="J8" s="8" t="n">
-        <v>53.20552127078303</v>
+        <v>51.44602482716887</v>
       </c>
       <c r="K8" t="n">
-        <v>56.54715548848657</v>
+        <v>57.89757356806936</v>
       </c>
       <c r="L8" s="8" t="n">
-        <v>2.703323529411662</v>
+        <v>3.2974705882352</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.8796652147920412</v>
+        <v>-2.10662777507698</v>
       </c>
       <c r="N8" t="n">
-        <v>96.84166666666668</v>
+        <v>104.405</v>
       </c>
       <c r="O8" t="n">
-        <v>133.875</v>
+        <v>128.99</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ATGL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APPL</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-TGL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PPL/financials-overview/</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-TGL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PPL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BERG</t>
+          <t>OGDC</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>STRONG_BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>78.13</v>
+        <v>133.13</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H9" t="n">
-        <v>243272</v>
+        <v>3920835</v>
       </c>
       <c r="I9" t="n">
-        <v>21.21899254831918</v>
+        <v>16.83098798182668</v>
       </c>
       <c r="J9" s="8" t="n">
-        <v>59.61951472937514</v>
+        <v>50.63045725658272</v>
       </c>
       <c r="K9" t="n">
-        <v>52.72079572331086</v>
+        <v>52.88804817439503</v>
       </c>
       <c r="L9" s="8" t="n">
-        <v>0.2789999999999822</v>
+        <v>1.973558823529515</v>
       </c>
       <c r="M9" t="n">
-        <v>3.16915357190016</v>
+        <v>-0.797317436661694</v>
       </c>
       <c r="N9" t="n">
-        <v>63.93444444444444</v>
+        <v>112.6672222222222</v>
       </c>
       <c r="O9" t="n">
-        <v>82.83611111111111</v>
+        <v>149.4988888888889</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ABERG</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AOGDC</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-BERG/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-OGDC/financials-overview/</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-BERG/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-OGDC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PPL</t>
+          <t>PHDL</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -5425,64 +5425,64 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>120.82</v>
+        <v>679.55</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G10" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" t="n">
-        <v>2447648</v>
+        <v>999980</v>
       </c>
       <c r="I10" t="n">
-        <v>17.79431331633835</v>
+        <v>43.50505576760017</v>
       </c>
       <c r="J10" s="8" t="n">
-        <v>51.44602482716887</v>
+        <v>81.64171160372202</v>
       </c>
       <c r="K10" t="n">
-        <v>57.89757356806936</v>
+        <v>88.13494446260752</v>
       </c>
       <c r="L10" s="8" t="n">
-        <v>3.2974705882352</v>
+        <v>147.250852941176</v>
       </c>
       <c r="M10" t="n">
-        <v>-2.10662777507698</v>
+        <v>-2.397161898196032</v>
       </c>
       <c r="N10" t="n">
-        <v>104.405</v>
+        <v>359.2011111111112</v>
       </c>
       <c r="O10" t="n">
-        <v>128.99</v>
+        <v>714.6844444444445</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APPL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APHDL</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PPL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PHDL/financials-overview/</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PPL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-PHDL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OGDC</t>
+          <t>EFERT</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -5491,130 +5491,130 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>133.13</v>
+        <v>167.68</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" t="n">
         <v>10</v>
       </c>
       <c r="G11" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="H11" t="n">
-        <v>3920835</v>
+        <v>343917</v>
       </c>
       <c r="I11" t="n">
-        <v>16.83098798182668</v>
+        <v>34.45297992055669</v>
       </c>
       <c r="J11" s="8" t="n">
-        <v>50.63045725658272</v>
+        <v>59.08768870734961</v>
       </c>
       <c r="K11" t="n">
-        <v>52.88804817439503</v>
+        <v>62.12765718104404</v>
       </c>
       <c r="L11" s="8" t="n">
-        <v>1.973558823529515</v>
+        <v>6.197911764705822</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.797317436661694</v>
+        <v>-0.5869449220371025</v>
       </c>
       <c r="N11" t="n">
-        <v>112.6672222222222</v>
+        <v>148.2594444444445</v>
       </c>
       <c r="O11" t="n">
-        <v>149.4988888888889</v>
+        <v>180.0127777777778</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AOGDC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AEFERT</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-OGDC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-EFERT/financials-overview/</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-OGDC/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-EFERT/technicals/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ATLH</t>
+          <t>MEBL</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>STRONG_BUY</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>665.92</v>
+        <v>237.99</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="H12" t="n">
-        <v>227283</v>
+        <v>569043</v>
       </c>
       <c r="I12" t="n">
-        <v>37.20957533611482</v>
+        <v>28.3289958800762</v>
       </c>
       <c r="J12" s="8" t="n">
-        <v>85.53275775253466</v>
+        <v>51.42893932756226</v>
       </c>
       <c r="K12" t="n">
-        <v>82.90426397979073</v>
+        <v>52.03850215953036</v>
       </c>
       <c r="L12" s="8" t="n">
-        <v>63.90150000000062</v>
+        <v>2.089764705882203</v>
       </c>
       <c r="M12" t="n">
-        <v>5.089399845345369</v>
+        <v>-0.1887267237040717</v>
       </c>
       <c r="N12" t="n">
-        <v>418.4155555555555</v>
+        <v>200.1077777777778</v>
       </c>
       <c r="O12" t="n">
-        <v>555.9155555555554</v>
+        <v>281.4894444444444</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AATLH</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMEBL</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-ATLH/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-MEBL/financials-overview/</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-ATLH/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-MEBL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PHDL</t>
+          <t>ISL</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -5623,64 +5623,64 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>679.55</v>
+        <v>87.93000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" t="n">
         <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>999980</v>
+        <v>550115</v>
       </c>
       <c r="I13" t="n">
-        <v>43.50505576760017</v>
+        <v>27.80052063545756</v>
       </c>
       <c r="J13" s="8" t="n">
-        <v>81.64171160372202</v>
+        <v>56.58005880182097</v>
       </c>
       <c r="K13" t="n">
-        <v>88.13494446260752</v>
+        <v>60.33427835050772</v>
       </c>
       <c r="L13" s="8" t="n">
-        <v>147.250852941176</v>
+        <v>3.150882352941139</v>
       </c>
       <c r="M13" t="n">
-        <v>-2.397161898196032</v>
+        <v>-1.490029128388974</v>
       </c>
       <c r="N13" t="n">
-        <v>359.2011111111112</v>
+        <v>73.03666666666668</v>
       </c>
       <c r="O13" t="n">
-        <v>714.6844444444445</v>
+        <v>95.11000000000003</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APHDL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AISL</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PHDL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-ISL/financials-overview/</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PHDL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-ISL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>EFERT</t>
+          <t>FABL</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -5689,196 +5689,196 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>167.68</v>
+        <v>55.09</v>
       </c>
       <c r="E14" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
         <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>343917</v>
+        <v>2522929</v>
       </c>
       <c r="I14" t="n">
-        <v>34.45297992055669</v>
+        <v>54.57212869177462</v>
       </c>
       <c r="J14" s="8" t="n">
-        <v>59.08768870734961</v>
+        <v>69.36352074681317</v>
       </c>
       <c r="K14" t="n">
-        <v>62.12765718104404</v>
+        <v>72.17193666552606</v>
       </c>
       <c r="L14" s="8" t="n">
-        <v>6.197911764705822</v>
+        <v>9.898764705882357</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.5869449220371025</v>
+        <v>-1.148394042705892</v>
       </c>
       <c r="N14" t="n">
-        <v>148.2594444444445</v>
+        <v>39.06888888888889</v>
       </c>
       <c r="O14" t="n">
-        <v>180.0127777777778</v>
+        <v>59.12555555555556</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AEFERT</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFABL</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-EFERT/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-FABL/financials-overview/</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-EFERT/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-FABL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AIRLINK</t>
+          <t>HUBC</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>STRONG_BUY</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>95.02</v>
+        <v>158.4</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F15" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G15" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H15" t="n">
-        <v>7374844</v>
+        <v>5305104</v>
       </c>
       <c r="I15" t="n">
-        <v>37.21791669539879</v>
+        <v>58.88081084235238</v>
       </c>
       <c r="J15" s="8" t="n">
-        <v>72.01405378178835</v>
+        <v>57.31227694172289</v>
       </c>
       <c r="K15" t="n">
-        <v>74.16751254660768</v>
+        <v>66.43923316434918</v>
       </c>
       <c r="L15" s="8" t="n">
-        <v>10.21114705882356</v>
+        <v>13.86532352941188</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.7209278027374336</v>
+        <v>-2.300622956886443</v>
       </c>
       <c r="N15" t="n">
-        <v>64.42222222222223</v>
+        <v>125.8144444444445</v>
       </c>
       <c r="O15" t="n">
-        <v>103.3438888888889</v>
+        <v>187.9644444444445</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AAIRLINK</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AHUBC</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-AIRLINK/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-HUBC/financials-overview/</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-AIRLINK/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-HUBC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>MEBL</t>
+          <t>INIL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NEUTRAL</t>
+          <t>BUY</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>237.99</v>
+        <v>212.76</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="H16" t="n">
-        <v>569043</v>
+        <v>1094158</v>
       </c>
       <c r="I16" t="n">
-        <v>28.3289958800762</v>
+        <v>45.18365101546745</v>
       </c>
       <c r="J16" s="8" t="n">
-        <v>51.42893932756226</v>
+        <v>64.74785426384507</v>
       </c>
       <c r="K16" t="n">
-        <v>52.03850215953036</v>
+        <v>70.68997228129695</v>
       </c>
       <c r="L16" s="8" t="n">
-        <v>2.089764705882203</v>
+        <v>18.72626470588261</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.1887267237040717</v>
+        <v>-2.300592368094788</v>
       </c>
       <c r="N16" t="n">
-        <v>200.1077777777778</v>
+        <v>162.2638888888889</v>
       </c>
       <c r="O16" t="n">
-        <v>281.4894444444444</v>
+        <v>219.1155555555556</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMEBL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AINIL</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-MEBL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-INIL/financials-overview/</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-MEBL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-INIL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ISL</t>
+          <t>LPL</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -5887,64 +5887,64 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>87.93000000000001</v>
+        <v>25.32</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H17" t="n">
-        <v>550115</v>
+        <v>514292</v>
       </c>
       <c r="I17" t="n">
-        <v>27.80052063545756</v>
+        <v>25.53321479488029</v>
       </c>
       <c r="J17" s="8" t="n">
-        <v>56.58005880182097</v>
+        <v>54.48698797847746</v>
       </c>
       <c r="K17" t="n">
-        <v>60.33427835050772</v>
+        <v>54.73457238592672</v>
       </c>
       <c r="L17" s="8" t="n">
-        <v>3.150882352941139</v>
+        <v>0.6018235294117602</v>
       </c>
       <c r="M17" t="n">
-        <v>-1.490029128388974</v>
+        <v>-0.07892659826361316</v>
       </c>
       <c r="N17" t="n">
-        <v>73.03666666666668</v>
+        <v>20.40888888888889</v>
       </c>
       <c r="O17" t="n">
-        <v>95.11000000000003</v>
+        <v>29.19055555555556</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AISL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ALPL</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-ISL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-LPL/financials-overview/</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-ISL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-LPL/technicals/</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FABL</t>
+          <t>BIPL</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -5953,384 +5953,54 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>55.09</v>
+        <v>24.6</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G18" t="n">
         <v>14</v>
       </c>
       <c r="H18" t="n">
-        <v>2522929</v>
+        <v>1110713</v>
       </c>
       <c r="I18" t="n">
-        <v>54.57212869177462</v>
+        <v>28.07645628925059</v>
       </c>
       <c r="J18" s="8" t="n">
-        <v>69.36352074681317</v>
+        <v>64.61014530611683</v>
       </c>
       <c r="K18" t="n">
-        <v>72.17193666552606</v>
+        <v>70.7378735992385</v>
       </c>
       <c r="L18" s="8" t="n">
-        <v>9.898764705882357</v>
+        <v>2.024617647058811</v>
       </c>
       <c r="M18" t="n">
-        <v>-1.148394042705892</v>
+        <v>-2.147971360381858</v>
       </c>
       <c r="N18" t="n">
-        <v>39.06888888888889</v>
+        <v>18.55666666666666</v>
       </c>
       <c r="O18" t="n">
-        <v>59.12555555555556</v>
+        <v>25.34</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFABL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ABIPL</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-FABL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-BIPL/financials-overview/</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-FABL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>HUBC</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>158.4</v>
-      </c>
-      <c r="E19" t="n">
-        <v>6</v>
-      </c>
-      <c r="F19" t="n">
-        <v>10</v>
-      </c>
-      <c r="G19" t="n">
-        <v>10</v>
-      </c>
-      <c r="H19" t="n">
-        <v>5305104</v>
-      </c>
-      <c r="I19" t="n">
-        <v>58.88081084235238</v>
-      </c>
-      <c r="J19" s="8" t="n">
-        <v>57.31227694172289</v>
-      </c>
-      <c r="K19" t="n">
-        <v>66.43923316434918</v>
-      </c>
-      <c r="L19" s="8" t="n">
-        <v>13.86532352941188</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-2.300622956886443</v>
-      </c>
-      <c r="N19" t="n">
-        <v>125.8144444444445</v>
-      </c>
-      <c r="O19" t="n">
-        <v>187.9644444444445</v>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AHUBC</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HUBC/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HUBC/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>INIL</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>212.76</v>
-      </c>
-      <c r="E20" t="n">
-        <v>3</v>
-      </c>
-      <c r="F20" t="n">
-        <v>9</v>
-      </c>
-      <c r="G20" t="n">
-        <v>14</v>
-      </c>
-      <c r="H20" t="n">
-        <v>1094158</v>
-      </c>
-      <c r="I20" t="n">
-        <v>45.18365101546745</v>
-      </c>
-      <c r="J20" s="8" t="n">
-        <v>64.74785426384507</v>
-      </c>
-      <c r="K20" t="n">
-        <v>70.68997228129695</v>
-      </c>
-      <c r="L20" s="8" t="n">
-        <v>18.72626470588261</v>
-      </c>
-      <c r="M20" t="n">
-        <v>-2.300592368094788</v>
-      </c>
-      <c r="N20" t="n">
-        <v>162.2638888888889</v>
-      </c>
-      <c r="O20" t="n">
-        <v>219.1155555555556</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AINIL</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-INIL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-INIL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>LPL</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>25.32</v>
-      </c>
-      <c r="E21" t="n">
-        <v>5</v>
-      </c>
-      <c r="F21" t="n">
-        <v>9</v>
-      </c>
-      <c r="G21" t="n">
-        <v>12</v>
-      </c>
-      <c r="H21" t="n">
-        <v>514292</v>
-      </c>
-      <c r="I21" t="n">
-        <v>25.53321479488029</v>
-      </c>
-      <c r="J21" s="8" t="n">
-        <v>54.48698797847746</v>
-      </c>
-      <c r="K21" t="n">
-        <v>54.73457238592672</v>
-      </c>
-      <c r="L21" s="8" t="n">
-        <v>0.6018235294117602</v>
-      </c>
-      <c r="M21" t="n">
-        <v>-0.07892659826361316</v>
-      </c>
-      <c r="N21" t="n">
-        <v>20.40888888888889</v>
-      </c>
-      <c r="O21" t="n">
-        <v>29.19055555555556</v>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ALPL</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-LPL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-LPL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>BIPL</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="E22" t="n">
-        <v>4</v>
-      </c>
-      <c r="F22" t="n">
-        <v>8</v>
-      </c>
-      <c r="G22" t="n">
-        <v>14</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1110713</v>
-      </c>
-      <c r="I22" t="n">
-        <v>28.07645628925059</v>
-      </c>
-      <c r="J22" s="8" t="n">
-        <v>64.61014530611683</v>
-      </c>
-      <c r="K22" t="n">
-        <v>70.7378735992385</v>
-      </c>
-      <c r="L22" s="8" t="n">
-        <v>2.024617647058811</v>
-      </c>
-      <c r="M22" t="n">
-        <v>-2.147971360381858</v>
-      </c>
-      <c r="N22" t="n">
-        <v>18.55666666666666</v>
-      </c>
-      <c r="O22" t="n">
-        <v>25.34</v>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ABIPL</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-BIPL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
           <t>https://www.tradingview.com/symbols/PSX-BIPL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>SAZEW</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>STRONG_BUY</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1134.42</v>
-      </c>
-      <c r="E23" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" t="n">
-        <v>7</v>
-      </c>
-      <c r="G23" t="n">
-        <v>17</v>
-      </c>
-      <c r="H23" t="n">
-        <v>3094488</v>
-      </c>
-      <c r="I23" t="n">
-        <v>47.62913771462846</v>
-      </c>
-      <c r="J23" s="8" t="n">
-        <v>86.47512910795623</v>
-      </c>
-      <c r="K23" t="n">
-        <v>84.97628066349709</v>
-      </c>
-      <c r="L23" s="8" t="n">
-        <v>156.6078235294119</v>
-      </c>
-      <c r="M23" t="n">
-        <v>3.715555230485116</v>
-      </c>
-      <c r="N23" t="n">
-        <v>690.2177777777778</v>
-      </c>
-      <c r="O23" t="n">
-        <v>933.4094444444444</v>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ASAZEW</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-SAZEW/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-SAZEW/technicals/</t>
         </is>
       </c>
     </row>
@@ -6356,7 +6026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6461,1255 +6131,199 @@
     </row>
     <row r="2">
       <c r="A2" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>KOHC</t>
+          <t>SITC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>277.67</v>
+        <v>312.41</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H2" t="n">
-        <v>586102</v>
+        <v>265</v>
       </c>
       <c r="I2" t="n">
-        <v>45.96840354445689</v>
+        <v>22.9393221422809</v>
       </c>
       <c r="J2" s="8" t="n">
-        <v>75.96599585177277</v>
+        <v>50.10627042764323</v>
       </c>
       <c r="K2" t="n">
-        <v>79.14158399414431</v>
+        <v>51.63959218797292</v>
       </c>
       <c r="L2" s="8" t="n">
-        <v>43.25955882352952</v>
+        <v>7.1487647058824</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.8321428571428514</v>
+        <v>-0.8222222222222143</v>
       </c>
       <c r="N2" t="n">
-        <v>194.6172222222222</v>
+        <v>251.2394444444444</v>
       </c>
       <c r="O2" t="n">
-        <v>282.6172222222222</v>
+        <v>403.4061111111111</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AKOHC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ASITC</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-KOHC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-SITC/financials-overview/</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-KOHC/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-SITC/technicals/</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CPHL</t>
+          <t>LUCK</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>31.95</v>
+        <v>910.45</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3" t="n">
         <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>1697677</v>
+        <v>70321</v>
       </c>
       <c r="I3" t="n">
-        <v>24.98440791809918</v>
+        <v>20.81187897231441</v>
       </c>
       <c r="J3" s="8" t="n">
-        <v>61.21963527856168</v>
+        <v>51.5434482072546</v>
       </c>
       <c r="K3" t="n">
-        <v>64.70382229713717</v>
+        <v>57.36016186382696</v>
       </c>
       <c r="L3" s="8" t="n">
-        <v>2.844176470588174</v>
+        <v>16.70129411764685</v>
       </c>
       <c r="M3" t="n">
-        <v>-1.510480887792844</v>
+        <v>-1.453651989435852</v>
       </c>
       <c r="N3" t="n">
-        <v>26.43444444444445</v>
+        <v>838.4505555555555</v>
       </c>
       <c r="O3" t="n">
-        <v>30.44944444444444</v>
+        <v>1003.450555555556</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ACPHL</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ALUCK</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-CPHL/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-LUCK/financials-overview/</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-CPHL/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-LUCK/technicals/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="n">
-        <v>45483.81409944977</v>
+        <v>45483.83657231266</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PABC</t>
+          <t>MEBL</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>75.98999999999999</v>
+        <v>237.99</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H4" t="n">
-        <v>1029315</v>
+        <v>569043</v>
       </c>
       <c r="I4" t="n">
-        <v>20.31190401707754</v>
+        <v>28.3289958800762</v>
       </c>
       <c r="J4" s="8" t="n">
-        <v>62.74527517100422</v>
+        <v>51.42893932756226</v>
       </c>
       <c r="K4" t="n">
-        <v>61.44243158837864</v>
+        <v>52.03850215953036</v>
       </c>
       <c r="L4" s="8" t="n">
-        <v>2.090647058823606</v>
+        <v>2.089764705882203</v>
       </c>
       <c r="M4" t="n">
-        <v>0.769128762763557</v>
+        <v>-0.1887267237040717</v>
       </c>
       <c r="N4" t="n">
-        <v>67.55555555555556</v>
+        <v>200.1077777777778</v>
       </c>
       <c r="O4" t="n">
-        <v>78.55555555555556</v>
+        <v>281.4894444444444</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APABC</t>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMEBL</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PABC/financials-overview/</t>
+          <t>https://www.tradingview.com/symbols/PSX-MEBL/financials-overview/</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>https://www.tradingview.com/symbols/PSX-PABC/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PAEL</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>25.49</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>10</v>
-      </c>
-      <c r="G5" t="n">
-        <v>11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>5599157</v>
-      </c>
-      <c r="I5" t="n">
-        <v>16.97528834220062</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>51.00091281209864</v>
-      </c>
-      <c r="K5" t="n">
-        <v>56.60698881510402</v>
-      </c>
-      <c r="L5" s="8" t="n">
-        <v>0.9227941176470438</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-2.337164750957866</v>
-      </c>
-      <c r="N5" t="n">
-        <v>22.30833333333334</v>
-      </c>
-      <c r="O5" t="n">
-        <v>27.27666666666667</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APAEL</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PAEL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PAEL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PIOC</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>178.75</v>
-      </c>
-      <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" t="n">
-        <v>14</v>
-      </c>
-      <c r="H6" t="n">
-        <v>118668</v>
-      </c>
-      <c r="I6" t="n">
-        <v>26.97168692097832</v>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v>66.43928143411412</v>
-      </c>
-      <c r="K6" t="n">
-        <v>70.81171884051835</v>
-      </c>
-      <c r="L6" s="8" t="n">
-        <v>14.27126470588234</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-1.237637438532521</v>
-      </c>
-      <c r="N6" t="n">
-        <v>135.0205555555556</v>
-      </c>
-      <c r="O6" t="n">
-        <v>188.9938888888889</v>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APIOC</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PIOC/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PIOC/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>OLPM</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>14</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>9</v>
-      </c>
-      <c r="G7" t="n">
-        <v>14</v>
-      </c>
-      <c r="H7" t="n">
-        <v>66527</v>
-      </c>
-      <c r="I7" t="n">
-        <v>20.59248510920501</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>55.06311559956592</v>
-      </c>
-      <c r="K7" t="n">
-        <v>55.06311559956592</v>
-      </c>
-      <c r="L7" s="8" t="n">
-        <v>0.4313823529411671</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>12.53222222222222</v>
-      </c>
-      <c r="O7" t="n">
-        <v>14.86055555555556</v>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AOLPM</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-OLPM/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-OLPM/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TGL</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>116.06</v>
-      </c>
-      <c r="E8" t="n">
-        <v>5</v>
-      </c>
-      <c r="F8" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" t="n">
-        <v>11</v>
-      </c>
-      <c r="H8" t="n">
-        <v>168359</v>
-      </c>
-      <c r="I8" t="n">
-        <v>37.321931890146</v>
-      </c>
-      <c r="J8" s="8" t="n">
-        <v>53.20552127078303</v>
-      </c>
-      <c r="K8" t="n">
-        <v>56.54715548848657</v>
-      </c>
-      <c r="L8" s="8" t="n">
-        <v>2.703323529411662</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-0.8796652147920412</v>
-      </c>
-      <c r="N8" t="n">
-        <v>96.84166666666668</v>
-      </c>
-      <c r="O8" t="n">
-        <v>133.875</v>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ATGL</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-TGL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-TGL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PPL</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>120.82</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-      <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="n">
-        <v>12</v>
-      </c>
-      <c r="H9" t="n">
-        <v>2447648</v>
-      </c>
-      <c r="I9" t="n">
-        <v>17.79431331633835</v>
-      </c>
-      <c r="J9" s="8" t="n">
-        <v>51.44602482716887</v>
-      </c>
-      <c r="K9" t="n">
-        <v>57.89757356806936</v>
-      </c>
-      <c r="L9" s="8" t="n">
-        <v>3.2974705882352</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-2.10662777507698</v>
-      </c>
-      <c r="N9" t="n">
-        <v>104.405</v>
-      </c>
-      <c r="O9" t="n">
-        <v>128.99</v>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APPL</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PPL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PPL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>OGDC</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>133.13</v>
-      </c>
-      <c r="E10" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" t="n">
-        <v>10</v>
-      </c>
-      <c r="G10" t="n">
-        <v>11</v>
-      </c>
-      <c r="H10" t="n">
-        <v>3920835</v>
-      </c>
-      <c r="I10" t="n">
-        <v>16.83098798182668</v>
-      </c>
-      <c r="J10" s="8" t="n">
-        <v>50.63045725658272</v>
-      </c>
-      <c r="K10" t="n">
-        <v>52.88804817439503</v>
-      </c>
-      <c r="L10" s="8" t="n">
-        <v>1.973558823529515</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-0.797317436661694</v>
-      </c>
-      <c r="N10" t="n">
-        <v>112.6672222222222</v>
-      </c>
-      <c r="O10" t="n">
-        <v>149.4988888888889</v>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AOGDC</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-OGDC/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-OGDC/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>FHAM</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14</v>
-      </c>
-      <c r="H11" t="n">
-        <v>15906</v>
-      </c>
-      <c r="I11" t="n">
-        <v>24.59580430098427</v>
-      </c>
-      <c r="J11" s="8" t="n">
-        <v>56.9578228376124</v>
-      </c>
-      <c r="K11" t="n">
-        <v>60.08914027669686</v>
-      </c>
-      <c r="L11" s="8" t="n">
-        <v>0.4724705882352929</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-0.6060606060606146</v>
-      </c>
-      <c r="N11" t="n">
-        <v>14.98944444444445</v>
-      </c>
-      <c r="O11" t="n">
-        <v>16.95111111111111</v>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFHAM</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-FHAM/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-FHAM/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PHDL</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>679.55</v>
-      </c>
-      <c r="E12" t="n">
-        <v>6</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" t="n">
-        <v>14</v>
-      </c>
-      <c r="H12" t="n">
-        <v>999980</v>
-      </c>
-      <c r="I12" t="n">
-        <v>43.50505576760017</v>
-      </c>
-      <c r="J12" s="8" t="n">
-        <v>81.64171160372202</v>
-      </c>
-      <c r="K12" t="n">
-        <v>88.13494446260752</v>
-      </c>
-      <c r="L12" s="8" t="n">
-        <v>147.250852941176</v>
-      </c>
-      <c r="M12" t="n">
-        <v>-2.397161898196032</v>
-      </c>
-      <c r="N12" t="n">
-        <v>359.2011111111112</v>
-      </c>
-      <c r="O12" t="n">
-        <v>714.6844444444445</v>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APHDL</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PHDL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-PHDL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>EFERT</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>167.68</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" t="n">
-        <v>10</v>
-      </c>
-      <c r="G13" t="n">
-        <v>13</v>
-      </c>
-      <c r="H13" t="n">
-        <v>343917</v>
-      </c>
-      <c r="I13" t="n">
-        <v>34.45297992055669</v>
-      </c>
-      <c r="J13" s="8" t="n">
-        <v>59.08768870734961</v>
-      </c>
-      <c r="K13" t="n">
-        <v>62.12765718104404</v>
-      </c>
-      <c r="L13" s="8" t="n">
-        <v>6.197911764705822</v>
-      </c>
-      <c r="M13" t="n">
-        <v>-0.5869449220371025</v>
-      </c>
-      <c r="N13" t="n">
-        <v>148.2594444444445</v>
-      </c>
-      <c r="O13" t="n">
-        <v>180.0127777777778</v>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AEFERT</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-EFERT/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-EFERT/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ISL</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>87.93000000000001</v>
-      </c>
-      <c r="E14" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" t="n">
-        <v>10</v>
-      </c>
-      <c r="G14" t="n">
-        <v>14</v>
-      </c>
-      <c r="H14" t="n">
-        <v>550115</v>
-      </c>
-      <c r="I14" t="n">
-        <v>27.80052063545756</v>
-      </c>
-      <c r="J14" s="8" t="n">
-        <v>56.58005880182097</v>
-      </c>
-      <c r="K14" t="n">
-        <v>60.33427835050772</v>
-      </c>
-      <c r="L14" s="8" t="n">
-        <v>3.150882352941139</v>
-      </c>
-      <c r="M14" t="n">
-        <v>-1.490029128388974</v>
-      </c>
-      <c r="N14" t="n">
-        <v>73.03666666666668</v>
-      </c>
-      <c r="O14" t="n">
-        <v>95.11000000000003</v>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AISL</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-ISL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-ISL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>FABL</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>55.09</v>
-      </c>
-      <c r="E15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F15" t="n">
-        <v>10</v>
-      </c>
-      <c r="G15" t="n">
-        <v>14</v>
-      </c>
-      <c r="H15" t="n">
-        <v>2522929</v>
-      </c>
-      <c r="I15" t="n">
-        <v>54.57212869177462</v>
-      </c>
-      <c r="J15" s="8" t="n">
-        <v>69.36352074681317</v>
-      </c>
-      <c r="K15" t="n">
-        <v>72.17193666552606</v>
-      </c>
-      <c r="L15" s="8" t="n">
-        <v>9.898764705882357</v>
-      </c>
-      <c r="M15" t="n">
-        <v>-1.148394042705892</v>
-      </c>
-      <c r="N15" t="n">
-        <v>39.06888888888889</v>
-      </c>
-      <c r="O15" t="n">
-        <v>59.12555555555556</v>
-      </c>
-      <c r="P15" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFABL</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-FABL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-FABL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HUBC</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>158.4</v>
-      </c>
-      <c r="E16" t="n">
-        <v>6</v>
-      </c>
-      <c r="F16" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" t="n">
-        <v>10</v>
-      </c>
-      <c r="H16" t="n">
-        <v>5305104</v>
-      </c>
-      <c r="I16" t="n">
-        <v>58.88081084235238</v>
-      </c>
-      <c r="J16" s="8" t="n">
-        <v>57.31227694172289</v>
-      </c>
-      <c r="K16" t="n">
-        <v>66.43923316434918</v>
-      </c>
-      <c r="L16" s="8" t="n">
-        <v>13.86532352941188</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-2.300622956886443</v>
-      </c>
-      <c r="N16" t="n">
-        <v>125.8144444444445</v>
-      </c>
-      <c r="O16" t="n">
-        <v>187.9644444444445</v>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AHUBC</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HUBC/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HUBC/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>INIL</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>212.76</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3</v>
-      </c>
-      <c r="F17" t="n">
-        <v>9</v>
-      </c>
-      <c r="G17" t="n">
-        <v>14</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1094158</v>
-      </c>
-      <c r="I17" t="n">
-        <v>45.18365101546745</v>
-      </c>
-      <c r="J17" s="8" t="n">
-        <v>64.74785426384507</v>
-      </c>
-      <c r="K17" t="n">
-        <v>70.68997228129695</v>
-      </c>
-      <c r="L17" s="8" t="n">
-        <v>18.72626470588261</v>
-      </c>
-      <c r="M17" t="n">
-        <v>-2.300592368094788</v>
-      </c>
-      <c r="N17" t="n">
-        <v>162.2638888888889</v>
-      </c>
-      <c r="O17" t="n">
-        <v>219.1155555555556</v>
-      </c>
-      <c r="P17" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AINIL</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-INIL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-INIL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>LPL</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>25.32</v>
-      </c>
-      <c r="E18" t="n">
-        <v>5</v>
-      </c>
-      <c r="F18" t="n">
-        <v>9</v>
-      </c>
-      <c r="G18" t="n">
-        <v>12</v>
-      </c>
-      <c r="H18" t="n">
-        <v>514292</v>
-      </c>
-      <c r="I18" t="n">
-        <v>25.53321479488029</v>
-      </c>
-      <c r="J18" s="8" t="n">
-        <v>54.48698797847746</v>
-      </c>
-      <c r="K18" t="n">
-        <v>54.73457238592672</v>
-      </c>
-      <c r="L18" s="8" t="n">
-        <v>0.6018235294117602</v>
-      </c>
-      <c r="M18" t="n">
-        <v>-0.07892659826361316</v>
-      </c>
-      <c r="N18" t="n">
-        <v>20.40888888888889</v>
-      </c>
-      <c r="O18" t="n">
-        <v>29.19055555555556</v>
-      </c>
-      <c r="P18" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ALPL</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-LPL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-LPL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>BIPL</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>24.6</v>
-      </c>
-      <c r="E19" t="n">
-        <v>4</v>
-      </c>
-      <c r="F19" t="n">
-        <v>8</v>
-      </c>
-      <c r="G19" t="n">
-        <v>14</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1110713</v>
-      </c>
-      <c r="I19" t="n">
-        <v>28.07645628925059</v>
-      </c>
-      <c r="J19" s="8" t="n">
-        <v>64.61014530611683</v>
-      </c>
-      <c r="K19" t="n">
-        <v>70.7378735992385</v>
-      </c>
-      <c r="L19" s="8" t="n">
-        <v>2.024617647058811</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-2.147971360381858</v>
-      </c>
-      <c r="N19" t="n">
-        <v>18.55666666666666</v>
-      </c>
-      <c r="O19" t="n">
-        <v>25.34</v>
-      </c>
-      <c r="P19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ABIPL</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-BIPL/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-BIPL/technicals/</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="n">
-        <v>45483.81409944977</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>HALEON</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>309.95</v>
-      </c>
-      <c r="E20" t="n">
-        <v>2</v>
-      </c>
-      <c r="F20" t="n">
-        <v>10</v>
-      </c>
-      <c r="G20" t="n">
-        <v>14</v>
-      </c>
-      <c r="H20" t="n">
-        <v>20569</v>
-      </c>
-      <c r="I20" t="n">
-        <v>19.26912944610719</v>
-      </c>
-      <c r="J20" s="8" t="n">
-        <v>65.30205081560976</v>
-      </c>
-      <c r="K20" t="n">
-        <v>64.83398111909142</v>
-      </c>
-      <c r="L20" s="8" t="n">
-        <v>27.61770588235282</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.3334196555742499</v>
-      </c>
-      <c r="N20" t="n">
-        <v>237.8538888888889</v>
-      </c>
-      <c r="O20" t="n">
-        <v>329.5388888888889</v>
-      </c>
-      <c r="P20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AHALEON</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HALEON/financials-overview/</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>https://www.tradingview.com/symbols/PSX-HALEON/technicals/</t>
+          <t>https://www.tradingview.com/symbols/PSX-MEBL/technicals/</t>
         </is>
       </c>
     </row>
@@ -7735,7 +6349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7835,6 +6449,534 @@
       <c r="R1" s="5" t="inlineStr">
         <is>
           <t>Technicals</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COLG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1189.71</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5679</v>
+      </c>
+      <c r="I2" t="n">
+        <v>45.39593336067106</v>
+      </c>
+      <c r="J2" s="8" t="n">
+        <v>30.08438758838442</v>
+      </c>
+      <c r="K2" t="n">
+        <v>28.61709904124322</v>
+      </c>
+      <c r="L2" s="8" t="n">
+        <v>-59.5661764705867</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.1894800666969835</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1061.721666666667</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1362.296666666666</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ACOLG</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-COLG/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-COLG/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MARI</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2670.93</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="n">
+        <v>11593</v>
+      </c>
+      <c r="I3" t="n">
+        <v>16.02204428480296</v>
+      </c>
+      <c r="J3" s="8" t="n">
+        <v>47.09431240523677</v>
+      </c>
+      <c r="K3" t="n">
+        <v>47.07712887498585</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>-13.04997058823756</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.00411858530337771</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2412.076666666667</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2941.91</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMARI</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MARI/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MARI/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MTL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>611.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>172411</v>
+      </c>
+      <c r="I4" t="n">
+        <v>26.87638166927452</v>
+      </c>
+      <c r="J4" s="8" t="n">
+        <v>37.44034964211425</v>
+      </c>
+      <c r="K4" t="n">
+        <v>47.06625156846526</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>-7.686529411765491</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-2.888786487216573</v>
+      </c>
+      <c r="N4" t="n">
+        <v>582.9072222222222</v>
+      </c>
+      <c r="O4" t="n">
+        <v>694.8138888888889</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMTL</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MTL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MTL/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>SGF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>68.28</v>
+      </c>
+      <c r="E5" t="n">
+        <v>12</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>118390</v>
+      </c>
+      <c r="I5" t="n">
+        <v>22.57557286226506</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>32.97182474853152</v>
+      </c>
+      <c r="K5" t="n">
+        <v>36.79022118626042</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>-6.402500000000046</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-2.289639381797359</v>
+      </c>
+      <c r="N5" t="n">
+        <v>65.24388888888889</v>
+      </c>
+      <c r="O5" t="n">
+        <v>89.88388888888888</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ASGF</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-SGF/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-SGF/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AGTL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>349.69</v>
+      </c>
+      <c r="E6" t="n">
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7270</v>
+      </c>
+      <c r="I6" t="n">
+        <v>14.99819040264111</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>45.66638905540498</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46.14819282235061</v>
+      </c>
+      <c r="L6" s="8" t="n">
+        <v>-2.385676470588749</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-0.08571673476385364</v>
+      </c>
+      <c r="N6" t="n">
+        <v>324.2377777777778</v>
+      </c>
+      <c r="O6" t="n">
+        <v>373.2427777777778</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AAGTL</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-AGTL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-AGTL/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>FRSM</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>50.51</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>22.55703789568202</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>36.16835577410773</v>
+      </c>
+      <c r="K7" t="n">
+        <v>36.16835577410773</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>-6.553999999999753</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>47.07333333333332</v>
+      </c>
+      <c r="O7" t="n">
+        <v>60.87833333333333</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFRSM</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-FRSM/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-FRSM/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>THALL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>430.02</v>
+      </c>
+      <c r="E8" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3531</v>
+      </c>
+      <c r="I8" t="n">
+        <v>24.80034541338028</v>
+      </c>
+      <c r="J8" s="8" t="n">
+        <v>43.66474251117698</v>
+      </c>
+      <c r="K8" t="n">
+        <v>47.97199637955811</v>
+      </c>
+      <c r="L8" s="8" t="n">
+        <v>-8.931411764705558</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-2.908105667193497</v>
+      </c>
+      <c r="N8" t="n">
+        <v>371.305</v>
+      </c>
+      <c r="O8" t="n">
+        <v>554.6199999999999</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ATHALL</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-THALL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-THALL/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>WTL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="n">
+        <v>9</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>20107488</v>
+      </c>
+      <c r="I9" t="n">
+        <v>14.14047160946565</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>41.27865559757308</v>
+      </c>
+      <c r="K9" t="n">
+        <v>38.72897597043073</v>
+      </c>
+      <c r="L9" s="8" t="n">
+        <v>-0.05591176470588288</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.8064516129032264</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.113333333333333</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.443333333333333</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AWTL</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-WTL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-WTL/technicals/</t>
         </is>
       </c>
     </row>
@@ -7860,7 +7002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7960,6 +7102,402 @@
       <c r="R1" s="5" t="inlineStr">
         <is>
           <t>Technicals</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MACTER</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STRONG_SELL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>90.04000000000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>616</v>
+      </c>
+      <c r="I2" t="n">
+        <v>10.31021067164274</v>
+      </c>
+      <c r="J2" s="8" t="n">
+        <v>44.02442756124596</v>
+      </c>
+      <c r="K2" t="n">
+        <v>43.91788806198672</v>
+      </c>
+      <c r="L2" s="8" t="n">
+        <v>1.558970588235255</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.04444444444445139</v>
+      </c>
+      <c r="N2" t="n">
+        <v>80.09111111111112</v>
+      </c>
+      <c r="O2" t="n">
+        <v>106.4361111111111</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AMACTER</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MACTER/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-MACTER/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ICL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>43.81</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8749</v>
+      </c>
+      <c r="I3" t="n">
+        <v>43.20108551771042</v>
+      </c>
+      <c r="J3" s="8" t="n">
+        <v>44.08503228640882</v>
+      </c>
+      <c r="K3" t="n">
+        <v>46.31294756481805</v>
+      </c>
+      <c r="L3" s="8" t="n">
+        <v>0.07426470588237066</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.8374830239927512</v>
+      </c>
+      <c r="N3" t="n">
+        <v>38.25444444444445</v>
+      </c>
+      <c r="O3" t="n">
+        <v>53.65444444444444</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AICL</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-ICL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-ICL/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CPPL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>118.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>21857</v>
+      </c>
+      <c r="I4" t="n">
+        <v>14.91398732271113</v>
+      </c>
+      <c r="J4" s="8" t="n">
+        <v>46.32608790503614</v>
+      </c>
+      <c r="K4" t="n">
+        <v>47.57385194845528</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>0.02867647058825185</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-0.4117993108664551</v>
+      </c>
+      <c r="N4" t="n">
+        <v>108.5983333333334</v>
+      </c>
+      <c r="O4" t="n">
+        <v>128.16</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ACPPL</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-CPPL/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-CPPL/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>FATIMA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>50.54</v>
+      </c>
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" t="n">
+        <v>9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" t="n">
+        <v>234766</v>
+      </c>
+      <c r="I5" t="n">
+        <v>25.02223926367896</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>48.4905882592903</v>
+      </c>
+      <c r="K5" t="n">
+        <v>56.299536361525</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>2.017558823529448</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-2.770296267795302</v>
+      </c>
+      <c r="N5" t="n">
+        <v>45.13</v>
+      </c>
+      <c r="O5" t="n">
+        <v>56.13</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3AFATIMA</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-FATIMA/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-FATIMA/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>PPP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>74.14</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>12088</v>
+      </c>
+      <c r="I6" t="n">
+        <v>12.93252690177482</v>
+      </c>
+      <c r="J6" s="8" t="n">
+        <v>49.7569378194056</v>
+      </c>
+      <c r="K6" t="n">
+        <v>54.75730307633658</v>
+      </c>
+      <c r="L6" s="8" t="n">
+        <v>1.918558823529395</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-1.82733050847457</v>
+      </c>
+      <c r="N6" t="n">
+        <v>68.18388888888889</v>
+      </c>
+      <c r="O6" t="n">
+        <v>81.43888888888888</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3APPP</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-PPP/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-PPP/technicals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="n">
+        <v>45483.83657231266</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SURC</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>130.06</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>243</v>
+      </c>
+      <c r="I7" t="n">
+        <v>13.74515278582335</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>43.95518810887903</v>
+      </c>
+      <c r="K7" t="n">
+        <v>48.87341950916313</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>1.909911764705896</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-2.364687335785606</v>
+      </c>
+      <c r="N7" t="n">
+        <v>120.1666666666667</v>
+      </c>
+      <c r="O7" t="n">
+        <v>153.1666666666667</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/chart/ZMYE714n/?symbol=PSX%3ASURC</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-SURC/financials-overview/</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>https://www.tradingview.com/symbols/PSX-SURC/technicals/</t>
         </is>
       </c>
     </row>

</xml_diff>